<commit_message>
ng: update onto forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2024/ng_oncho_2026_2_river_inspection.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2024/ng_oncho_2026_2_river_inspection.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A16A1C11-CBCD-4B24-BBAB-0903DF1BAC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8AEB3-5128-4ED3-9FA5-1E114EDA4D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="158">
   <si>
     <t>type</t>
   </si>
@@ -356,12 +356,6 @@
   </si>
   <si>
     <t>State</t>
-  </si>
-  <si>
-    <t>ng_oncho_2026_2_river_inspection</t>
-  </si>
-  <si>
-    <t>2. River inspection Form</t>
   </si>
   <si>
     <t>lga</t>
@@ -509,6 +503,18 @@
   </si>
   <si>
     <t>River calm/slow flow</t>
+  </si>
+  <si>
+    <t>not(selected(${river_details}, 'River.rapids/fast.flow') and selected(${river_details}, 'River.calm/slow.flow'))</t>
+  </si>
+  <si>
+    <t>The river cannot be fast and slow at the same time</t>
+  </si>
+  <si>
+    <t>ng_oncho_2026_2_river_inspection_v2</t>
+  </si>
+  <si>
+    <t>2. River inspection Form V2</t>
   </si>
 </sst>
 </file>
@@ -1045,10 +1051,10 @@
   <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H24" sqref="H24"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1064,7 @@
     <col min="3" max="3" width="44.875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.75" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="43.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="29.5" style="3" customWidth="1"/>
     <col min="8" max="8" width="29.75" style="3" customWidth="1"/>
     <col min="9" max="9" width="12.625" style="3" customWidth="1"/>
@@ -1142,7 +1148,7 @@
         <v>105</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>106</v>
@@ -1165,7 +1171,7 @@
         <v>105</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>78</v>
@@ -1187,7 +1193,7 @@
         <v>105</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>104</v>
@@ -1311,10 +1317,10 @@
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1417,7 +1423,7 @@
         <v>101</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
@@ -1442,7 +1448,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
@@ -1467,7 +1473,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
       <c r="H16" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
@@ -1517,7 +1523,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="9"/>
       <c r="H18" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
@@ -1588,7 +1594,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
       <c r="H21" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1611,7 +1617,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="9"/>
       <c r="H22" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1634,7 +1640,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="9"/>
       <c r="H23" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1644,22 +1650,22 @@
     </row>
     <row r="24" spans="1:13" s="10" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="9"/>
       <c r="H24" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1667,22 +1673,26 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="9"/>
+      <c r="F25" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>155</v>
+      </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7" t="s">
@@ -1694,16 +1704,16 @@
     </row>
     <row r="26" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1719,7 +1729,7 @@
     </row>
     <row r="27" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -1778,7 +1788,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="7"/>
@@ -1864,9 +1874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:A20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1887,10 +1897,10 @@
         <v>18</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1953,10 +1963,10 @@
         <v>76</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
@@ -1964,10 +1974,10 @@
         <v>76</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1986,10 +1996,10 @@
         <v>76</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2038,134 +2048,134 @@
     </row>
     <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C27" s="22" t="s">
         <v>140</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2780,7 +2790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2805,10 +2815,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
ng: update the oncho forms
</commit_message>
<xml_diff>
--- a/ONCHO/Entomological survey Survey/Nigeria/2024/ng_oncho_2026_2_river_inspection.xlsx
+++ b/ONCHO/Entomological survey Survey/Nigeria/2024/ng_oncho_2026_2_river_inspection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\ONCHO\Entomological survey Survey\Nigeria\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA8AEB3-5128-4ED3-9FA5-1E114EDA4D7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA76354-FD54-4CE4-B5DA-00822E9C4387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="252">
   <si>
     <t>type</t>
   </si>
@@ -350,9 +350,6 @@
   </si>
   <si>
     <t>Enter the Community Name</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>State</t>
@@ -511,10 +508,295 @@
     <t>The river cannot be fast and slow at the same time</t>
   </si>
   <si>
-    <t>ng_oncho_2026_2_river_inspection_v2</t>
-  </si>
-  <si>
-    <t>2. River inspection Form V2</t>
+    <t>ng_oncho_2026_2_river_insp_bau</t>
+  </si>
+  <si>
+    <t>(Bauchi) 2. River inspection Form</t>
+  </si>
+  <si>
+    <t>BAUCHI</t>
+  </si>
+  <si>
+    <t>ALKALERI</t>
+  </si>
+  <si>
+    <t>BOGORO</t>
+  </si>
+  <si>
+    <t>DARAZO</t>
+  </si>
+  <si>
+    <t>DASS</t>
+  </si>
+  <si>
+    <t>GAMAWA</t>
+  </si>
+  <si>
+    <t>GANJUWA</t>
+  </si>
+  <si>
+    <t>KIRFI</t>
+  </si>
+  <si>
+    <t>MISAU</t>
+  </si>
+  <si>
+    <t>NINGI</t>
+  </si>
+  <si>
+    <t>SHIRA</t>
+  </si>
+  <si>
+    <t>TORO</t>
+  </si>
+  <si>
+    <t>ZAKI</t>
+  </si>
+  <si>
+    <t>GIADE</t>
+  </si>
+  <si>
+    <t>TAFAWA-BALEWA</t>
+  </si>
+  <si>
+    <t>WARJI</t>
+  </si>
+  <si>
+    <t>community</t>
+  </si>
+  <si>
+    <t>BAKUREJI</t>
+  </si>
+  <si>
+    <t>DAGARAU</t>
+  </si>
+  <si>
+    <t>KWALA</t>
+  </si>
+  <si>
+    <t>YELWAN GALAMBI</t>
+  </si>
+  <si>
+    <t>BIRIM</t>
+  </si>
+  <si>
+    <t>MIRI</t>
+  </si>
+  <si>
+    <t>DOGON KANIA</t>
+  </si>
+  <si>
+    <t>SABON GARI</t>
+  </si>
+  <si>
+    <t>DARRARI</t>
+  </si>
+  <si>
+    <t>LIRINI</t>
+  </si>
+  <si>
+    <t>DADINGA</t>
+  </si>
+  <si>
+    <t>MIYA B</t>
+  </si>
+  <si>
+    <t>NASARAWA</t>
+  </si>
+  <si>
+    <t>CHINKANI</t>
+  </si>
+  <si>
+    <t>BARA</t>
+  </si>
+  <si>
+    <t>BUNDURU</t>
+  </si>
+  <si>
+    <t>FAFAN FULANI</t>
+  </si>
+  <si>
+    <t>ZINDI/MISAU</t>
+  </si>
+  <si>
+    <t>KAFIN LEMO</t>
+  </si>
+  <si>
+    <t>KAFIN ZAKI</t>
+  </si>
+  <si>
+    <t>RAFIN CHIAWO</t>
+  </si>
+  <si>
+    <t>SAMA</t>
+  </si>
+  <si>
+    <t>UNGUWAR MADAIKI</t>
+  </si>
+  <si>
+    <t>BANGIRE</t>
+  </si>
+  <si>
+    <t>DINDIBUS</t>
+  </si>
+  <si>
+    <t>DISINA B</t>
+  </si>
+  <si>
+    <t>ZIGAU</t>
+  </si>
+  <si>
+    <t>KARDAM B</t>
+  </si>
+  <si>
+    <t>GUMAU</t>
+  </si>
+  <si>
+    <t>LAME</t>
+  </si>
+  <si>
+    <t>RISHI</t>
+  </si>
+  <si>
+    <t>RUHU</t>
+  </si>
+  <si>
+    <t>GABANGA A</t>
+  </si>
+  <si>
+    <t>SANDIGALOU</t>
+  </si>
+  <si>
+    <t>TIKIRZE</t>
+  </si>
+  <si>
+    <t>BAU_ALK_N_001</t>
+  </si>
+  <si>
+    <t>BAU_ALK_N_002</t>
+  </si>
+  <si>
+    <t>BAU_ALK_N_003</t>
+  </si>
+  <si>
+    <t>BAU_BAU_N_004</t>
+  </si>
+  <si>
+    <t>BAU_BAU_N_005</t>
+  </si>
+  <si>
+    <t>BAU_BOG_N_006</t>
+  </si>
+  <si>
+    <t>BAU_DAR_N_007</t>
+  </si>
+  <si>
+    <t>BAU_DAS_N_008</t>
+  </si>
+  <si>
+    <t>BAU_GAM_N_009</t>
+  </si>
+  <si>
+    <t>BAU_GAM_N_010</t>
+  </si>
+  <si>
+    <t>BAU_GAM_N_011</t>
+  </si>
+  <si>
+    <t>BAU_GAM_N_012</t>
+  </si>
+  <si>
+    <t>BAU_KIR_N_013</t>
+  </si>
+  <si>
+    <t>BAU_KIR_N_014</t>
+  </si>
+  <si>
+    <t>BAU_MIS_N_015</t>
+  </si>
+  <si>
+    <t>BAU_NIN_N_016</t>
+  </si>
+  <si>
+    <t>BAU_NIN_N_017</t>
+  </si>
+  <si>
+    <t>BAU_NIN_N_018</t>
+  </si>
+  <si>
+    <t>BAU_NIN_N_019</t>
+  </si>
+  <si>
+    <t>BAU_SHI_N_020</t>
+  </si>
+  <si>
+    <t>BAU_TOR_N_021</t>
+  </si>
+  <si>
+    <t>BAU_TOR_N_022</t>
+  </si>
+  <si>
+    <t>BAU_TOR_N_023</t>
+  </si>
+  <si>
+    <t>BAU_TOR_N_024</t>
+  </si>
+  <si>
+    <t>BAU_ZAK_N_025</t>
+  </si>
+  <si>
+    <t>BAU_ZAK_N_026</t>
+  </si>
+  <si>
+    <t>BAU_KIR_M_027</t>
+  </si>
+  <si>
+    <t>BAU_ALK_M_028</t>
+  </si>
+  <si>
+    <t>BAU_GIA_M_029</t>
+  </si>
+  <si>
+    <t>BAU_GAN_M_030</t>
+  </si>
+  <si>
+    <t>BAU_NIN_M_031</t>
+  </si>
+  <si>
+    <t>BAU_SHI_M_032</t>
+  </si>
+  <si>
+    <t>BAU_TAF_M_033</t>
+  </si>
+  <si>
+    <t>BAU_SHI_M_034</t>
+  </si>
+  <si>
+    <t>BAU_WAR_M_035</t>
+  </si>
+  <si>
+    <t>BAU_SHI_M_036</t>
+  </si>
+  <si>
+    <t>select_one state</t>
+  </si>
+  <si>
+    <t>select_one lga</t>
+  </si>
+  <si>
+    <t>select_one community</t>
+  </si>
+  <si>
+    <t>select_one site_id</t>
+  </si>
+  <si>
+    <t>state = ${r_state}</t>
+  </si>
+  <si>
+    <t>lga = ${r_lga}</t>
+  </si>
+  <si>
+    <t>community = ${r_community}</t>
   </si>
 </sst>
 </file>
@@ -1050,11 +1332,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1145,13 +1427,13 @@
     </row>
     <row r="3" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>106</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="7"/>
@@ -1168,10 +1450,10 @@
     </row>
     <row r="4" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>246</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>78</v>
@@ -1186,14 +1468,17 @@
         <v>9</v>
       </c>
       <c r="K4" s="7"/>
+      <c r="L4" s="10" t="s">
+        <v>249</v>
+      </c>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>247</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>104</v>
@@ -1208,11 +1493,14 @@
         <v>9</v>
       </c>
       <c r="K5" s="7"/>
+      <c r="L5" s="10" t="s">
+        <v>250</v>
+      </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>248</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>38</v>
@@ -1230,7 +1518,9 @@
         <v>9</v>
       </c>
       <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="10" t="s">
+        <v>251</v>
+      </c>
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -1317,10 +1607,10 @@
       <c r="D10" s="9"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>113</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>114</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -1423,7 +1713,7 @@
         <v>101</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7" t="s">
@@ -1448,7 +1738,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7" t="s">
@@ -1473,7 +1763,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
       <c r="H16" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7" t="s">
@@ -1523,7 +1813,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="9"/>
       <c r="H18" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7" t="s">
@@ -1594,7 +1884,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="9"/>
       <c r="H21" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1617,7 +1907,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="9"/>
       <c r="H22" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1640,7 +1930,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="9"/>
       <c r="H23" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1650,22 +1940,22 @@
     </row>
     <row r="24" spans="1:13" s="10" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>119</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="9"/>
       <c r="H24" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1675,23 +1965,23 @@
     </row>
     <row r="25" spans="1:13" s="10" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>154</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>155</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -1704,16 +1994,16 @@
     </row>
     <row r="26" spans="1:13" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -1729,7 +2019,7 @@
     </row>
     <row r="27" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
@@ -1788,7 +2078,7 @@
         <v>90</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="7"/>
@@ -1872,11 +2162,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E170"/>
+  <dimension ref="A1:F170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1886,7 +2176,7 @@
     <col min="3" max="3" width="21.625" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
@@ -1897,13 +2187,16 @@
         <v>18</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +2207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -1925,7 +2218,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1936,7 +2229,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
@@ -1947,7 +2240,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -1958,29 +2251,29 @@
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>76</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>76</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>76</v>
       </c>
@@ -1991,18 +2284,18 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>76</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -2013,7 +2306,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -2024,7 +2317,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2035,7 +2328,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>84</v>
       </c>
@@ -2048,134 +2341,134 @@
     </row>
     <row r="18" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>126</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>89</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="22" t="s">
         <v>152</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C26" s="22" t="s">
         <v>138</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B27" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -2183,432 +2476,1277 @@
       <c r="C31" s="21"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
+      <c r="A32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="20"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="20"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="20"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="20"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="20"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="20"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="21"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B35" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="D38" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C39" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="C40" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C41" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B43" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="D43" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="C45" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="D46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B47" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C47" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D47" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="D48" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="C49" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="D49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="21"/>
       <c r="C50" s="21"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="21"/>
-      <c r="C51" s="21"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
-      <c r="B52" s="21"/>
-      <c r="C52" s="21"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="21"/>
-      <c r="C53" s="21"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="21"/>
-      <c r="C54" s="21"/>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="21"/>
-      <c r="C55" s="21"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="21"/>
-      <c r="C56" s="21"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="21"/>
-      <c r="C57" s="21"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="20"/>
-      <c r="B58" s="21"/>
-      <c r="C58" s="21"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="20"/>
-      <c r="B59" s="21"/>
-      <c r="C59" s="21"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="20"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="21"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
-      <c r="B61" s="21"/>
-      <c r="C61" s="21"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="20"/>
-      <c r="B62" s="21"/>
-      <c r="C62" s="21"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="21"/>
-      <c r="C63" s="21"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="21"/>
-      <c r="C64" s="21"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="20"/>
-      <c r="B66" s="21"/>
-      <c r="C66" s="21"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="21"/>
-      <c r="C67" s="21"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="21"/>
-      <c r="C68" s="21"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="21"/>
-      <c r="C69" s="21"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="21"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="21"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="21"/>
-      <c r="C72" s="21"/>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="21"/>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="21"/>
-      <c r="C74" s="21"/>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="21"/>
-      <c r="C75" s="21"/>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="21"/>
-      <c r="C76" s="21"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="21"/>
-      <c r="C77" s="21"/>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="21"/>
-      <c r="C78" s="21"/>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="21"/>
-      <c r="C79" s="21"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="21"/>
-      <c r="C80" s="21"/>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="21"/>
-      <c r="C81" s="21"/>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="21"/>
-      <c r="C82" s="21"/>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="21"/>
-      <c r="C83" s="21"/>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="21"/>
-      <c r="C84" s="21"/>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="21"/>
-      <c r="C86" s="21"/>
-    </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>173</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="C51" s="21" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>173</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>173</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="E54" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E55" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="E56" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>180</v>
+      </c>
+      <c r="E57" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E59" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="E60" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>173</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="E61" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="E62" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>173</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="E63" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="E64" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E65" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>173</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="E66" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>173</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E67" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>173</v>
+      </c>
+      <c r="B68" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="E68" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>173</v>
+      </c>
+      <c r="B69" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="C69" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="E69" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="E70" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>173</v>
+      </c>
+      <c r="B72" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="E72" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>173</v>
+      </c>
+      <c r="B73" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="C73" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="E74" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>173</v>
+      </c>
+      <c r="B75" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="E75" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>173</v>
+      </c>
+      <c r="B76" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="C76" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="E76" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>173</v>
+      </c>
+      <c r="B77" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="E77" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>173</v>
+      </c>
+      <c r="B78" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="E78" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>173</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="E79" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>173</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="E80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>173</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="E81" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>173</v>
+      </c>
+      <c r="B82" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>204</v>
+      </c>
+      <c r="E82" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>173</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E83" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>173</v>
+      </c>
+      <c r="B84" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E84" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>173</v>
+      </c>
+      <c r="B85" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="E85" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="E86" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B87" s="21"/>
       <c r="C87" s="21"/>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="21"/>
-      <c r="C88" s="21"/>
-    </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="21"/>
-      <c r="C89" s="21"/>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="21"/>
-      <c r="C90" s="21"/>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="21"/>
-      <c r="C91" s="21"/>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="21"/>
-      <c r="C93" s="21"/>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="21"/>
-      <c r="C94" s="21"/>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="21"/>
-      <c r="C95" s="21"/>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="21"/>
-      <c r="C96" s="21"/>
-    </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="21"/>
-      <c r="C97" s="21"/>
-    </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="21"/>
-      <c r="C98" s="21"/>
-    </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="21"/>
-      <c r="C99" s="21"/>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="21"/>
-      <c r="C100" s="21"/>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="21"/>
-      <c r="C101" s="21"/>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="21"/>
-      <c r="C102" s="21"/>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="21"/>
-      <c r="C103" s="21"/>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="21"/>
-      <c r="C104" s="21"/>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="21"/>
-      <c r="C105" s="21"/>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="21"/>
-      <c r="C106" s="21"/>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="21"/>
-      <c r="C107" s="21"/>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="21"/>
-      <c r="C108" s="21"/>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="21"/>
-      <c r="C109" s="21"/>
-    </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="21"/>
-      <c r="C110" s="21"/>
-    </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="21"/>
-      <c r="C111" s="21"/>
-    </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="21"/>
-      <c r="C112" s="21"/>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B113" s="21"/>
-      <c r="C113" s="21"/>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B114" s="21"/>
-      <c r="C114" s="21"/>
-    </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B115" s="21"/>
-      <c r="C115" s="21"/>
-    </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B116" s="21"/>
-      <c r="C116" s="21"/>
-    </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B117" s="21"/>
-      <c r="C117" s="21"/>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="21"/>
-      <c r="C118" s="21"/>
-    </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="21"/>
-      <c r="C119" s="21"/>
-    </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="21"/>
-      <c r="C120" s="21"/>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="21"/>
-      <c r="C121" s="21"/>
-    </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B122" s="21"/>
-      <c r="C122" s="21"/>
-    </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B123" s="21"/>
-      <c r="C123" s="21"/>
-    </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B88" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F88" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B89" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="F89" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B90" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="F90" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B91" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="F91" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B92" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="F92" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B93" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>214</v>
+      </c>
+      <c r="F93" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B94" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>215</v>
+      </c>
+      <c r="F94" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B95" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>216</v>
+      </c>
+      <c r="F95" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B96" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F96" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B97" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="F97" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B98" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>219</v>
+      </c>
+      <c r="F98" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B99" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="F99" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B100" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="F100" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="F101" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B102" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C102" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F102" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B103" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="C103" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="F103" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B104" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="C104" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="F104" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B105" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="C105" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="F105" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B106" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="C106" s="21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F106" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B107" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B108" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C108" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="F108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B109" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="F109" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B110" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="F110" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B111" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="F111" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B112" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="F112" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B113" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="C113" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="F113" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B114" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="C114" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="F114" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B115" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="F115" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B116" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="C116" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="F116" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B117" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="F117" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B118" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="C118" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="F118" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B119" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="F119" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B120" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="F120" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B121" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F121" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B122" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="C122" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F122" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B123" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C123" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="F123" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B124" s="21"/>
       <c r="C124" s="21"/>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B125" s="21"/>
       <c r="C125" s="21"/>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B126" s="21"/>
       <c r="C126" s="21"/>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B127" s="21"/>
       <c r="C127" s="21"/>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B128" s="21"/>
       <c r="C128" s="21"/>
     </row>
@@ -2790,8 +3928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2815,10 +3953,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>

</xml_diff>